<commit_message>
Added May agenda sheet
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@852 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Agendas/201301 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201301 WGM FHIR Agenda.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="8625" yWindow="600" windowWidth="16785" windowHeight="12810"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual" iterate="1" iterateCount="50"/>
 </workbook>
 </file>
 
@@ -327,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +337,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -371,6 +377,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,13 +683,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,11 +789,11 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="M3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -805,8 +815,8 @@
       <c r="H4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>37</v>
+      <c r="M4" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1020,6 +1030,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1032,6 +1043,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>